<commit_message>
Add problem statement and SQL scripts for tracking student performance improvements
</commit_message>
<xml_diff>
--- a/Student_Performance/Problem_Statement.xlsx
+++ b/Student_Performance/Problem_Statement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thoufiq/THOUFIQ/techTFQ/YouTube/VIDEOS/30 SQL Interview Queries/Video_Q6/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\30DaySQLQueryChallenge - techTFQ\Student_Performance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C87F994A-F0D1-6940-BC0B-F03387CD127F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46E365DA-BAC7-4B5C-A75F-E1B3A3C4BEE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{676511AD-201D-B74F-BBAA-90083F34A7EA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{676511AD-201D-B74F-BBAA-90083F34A7EA}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -42,30 +40,6 @@
   </si>
   <si>
     <t>MARKS</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <u/>
-        <sz val="14"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">VIDEO #6 </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>- Student Performance</t>
-    </r>
   </si>
   <si>
     <t>INPUT</t>
@@ -101,6 +75,30 @@
   </si>
   <si>
     <t>OUTPUT - 2</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <u/>
+        <sz val="14"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"># </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>- Student Performance</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -346,33 +344,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -381,12 +366,24 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -729,255 +726,251 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BA1ABCF-6E39-A746-B912-8E414A3D63A8}">
   <dimension ref="B1:N17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2:J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="7"/>
-    <col min="2" max="3" width="12.83203125" style="7" customWidth="1"/>
-    <col min="4" max="5" width="10.83203125" style="7"/>
-    <col min="6" max="7" width="12.83203125" style="7" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="7"/>
-    <col min="9" max="10" width="12.83203125" style="7" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="7"/>
+    <col min="2" max="3" width="12.796875" customWidth="1"/>
+    <col min="6" max="7" width="12.796875" customWidth="1"/>
+    <col min="9" max="10" width="12.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.2">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="2:14" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+      <c r="B1" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+    </row>
+    <row r="2" spans="2:14" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+    </row>
+    <row r="3" spans="2:14" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+    </row>
+    <row r="4" spans="2:14" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+    </row>
+    <row r="5" spans="2:14" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+    </row>
+    <row r="6" spans="2:14" s="1" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+    </row>
+    <row r="7" spans="2:14" s="1" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+    </row>
+    <row r="8" spans="2:14" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+    </row>
+    <row r="9" spans="2:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="2:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-    </row>
-    <row r="2" spans="2:14" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="4" t="s">
+      <c r="C10" s="22"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-    </row>
-    <row r="3" spans="2:14" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-    </row>
-    <row r="4" spans="2:14" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-    </row>
-    <row r="5" spans="2:14" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-    </row>
-    <row r="6" spans="2:14" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-    </row>
-    <row r="7" spans="2:14" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-    </row>
-    <row r="8" spans="2:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-    </row>
-    <row r="9" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="24" t="s">
+      <c r="G10" s="24"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="G10" s="25"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="J10" s="25"/>
-    </row>
-    <row r="11" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="16" t="s">
+      <c r="J10" s="24"/>
+    </row>
+    <row r="11" spans="2:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="G11" s="17" t="s">
+      <c r="G11" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="I11" s="16" t="s">
+      <c r="I11" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="J11" s="17" t="s">
+      <c r="J11" s="12" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B12" s="14">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B12" s="9">
         <v>100</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="10">
         <v>55</v>
       </c>
-      <c r="F12" s="22">
+      <c r="F12" s="17">
         <v>100</v>
       </c>
-      <c r="G12" s="23">
+      <c r="G12" s="18">
         <v>55</v>
       </c>
-      <c r="I12" s="22">
+      <c r="I12" s="17">
         <v>102</v>
       </c>
-      <c r="J12" s="23">
+      <c r="J12" s="18">
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="8">
+    <row r="13" spans="2:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="5">
         <v>101</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="6">
         <v>55</v>
       </c>
-      <c r="F13" s="18">
+      <c r="F13" s="13">
         <v>102</v>
       </c>
-      <c r="G13" s="19">
+      <c r="G13" s="14">
         <v>60</v>
       </c>
-      <c r="I13" s="20">
+      <c r="I13" s="15">
         <v>105</v>
       </c>
-      <c r="J13" s="21">
+      <c r="J13" s="16">
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="8">
+    <row r="14" spans="2:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="5">
         <v>102</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="6">
         <v>60</v>
       </c>
-      <c r="F14" s="20">
+      <c r="F14" s="15">
         <v>105</v>
       </c>
-      <c r="G14" s="21">
+      <c r="G14" s="16">
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B15" s="8">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B15" s="5">
         <v>103</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="6">
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B16" s="8">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B16" s="5">
         <v>104</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="6">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="2:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="10">
+    <row r="17" spans="2:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="7">
         <v>105</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C17" s="8">
         <v>50</v>
       </c>
     </row>
@@ -990,5 +983,6 @@
     <mergeCell ref="I10:J10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>